<commit_message>
Updated ProfileValidator class to process multiple profile worksheets. Removed a lot of unnecessary code. Updated sample profile to include multiple worksheets and an overview and namespaces worksheet
</commit_message>
<xml_diff>
--- a/examples/Schematron_Example_Profile.xlsx
+++ b/examples/Schematron_Example_Profile.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="18195" windowHeight="12270"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="18192" windowHeight="12216"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Overview" sheetId="5" r:id="rId1"/>
+    <sheet name="STIX Package" sheetId="3" r:id="rId2"/>
+    <sheet name="STIX Header" sheetId="6" r:id="rId3"/>
+    <sheet name="TTP" sheetId="7" r:id="rId4"/>
+    <sheet name="Namespaces" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>@idref</t>
   </si>
@@ -110,13 +114,120 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>http://stix.mitre.org/stix-1</t>
+  </si>
+  <si>
+    <t>stix</t>
+  </si>
+  <si>
+    <t>http://stix.mitre.org/common-1</t>
+  </si>
+  <si>
+    <t>stixCommon</t>
+  </si>
+  <si>
+    <t>http://stix.mitre.org/default_vocabularies-1</t>
+  </si>
+  <si>
+    <t>stixVocabs</t>
+  </si>
+  <si>
+    <t>Profile Information</t>
+  </si>
+  <si>
+    <t>Status: SAMPLE</t>
+  </si>
+  <si>
+    <r>
+      <t>Version:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> r1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Contact:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The MITRE Corporation (stix@mitre.org)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Distribution: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Public</t>
+    </r>
+  </si>
+  <si>
+    <t>Title: Example</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Date: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5 March 2014</t>
+    </r>
+  </si>
+  <si>
+    <t>http://www.w3.org/2001/XMLSchema-instance</t>
+  </si>
+  <si>
+    <t>xsi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +274,38 @@
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,15 +393,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -292,11 +436,16 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Required" xfId="5"/>
@@ -598,20 +747,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -637,7 +845,7 @@
       </c>
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -648,7 +856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -659,7 +867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -670,7 +878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -681,7 +889,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -692,7 +900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -703,7 +911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -714,7 +922,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -725,7 +933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -736,7 +944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
@@ -747,7 +955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
@@ -758,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
@@ -770,102 +978,248 @@
       </c>
       <c r="E14" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added some additional test values to profile
</commit_message>
<xml_diff>
--- a/examples/Schematron_Example_Profile.xlsx
+++ b/examples/Schematron_Example_Profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="18192" windowHeight="12216"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="18192" windowHeight="12216" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>prohibited</t>
   </si>
   <si>
-    <t>stixVocabs:PackageIntentVocab-1.0</t>
-  </si>
-  <si>
     <t>XPATH</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
   </si>
   <si>
     <t>stix:Observables</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
   <si>
     <t>Namespace</t>
@@ -221,6 +215,12 @@
   </si>
   <si>
     <t>xsi</t>
+  </si>
+  <si>
+    <t>1.0, 1.0.1</t>
+  </si>
+  <si>
+    <t>stixVocabs:PackageIntentVocab-1.0, stixVocabs:HighMediumLowVocab-1.0</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -760,37 +760,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
@@ -809,7 +809,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,7 +827,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>9</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>6</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>6</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>6</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>6</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>6</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>6</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>6</v>
@@ -977,7 +977,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>9</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>7</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>7</v>
@@ -1049,12 +1049,12 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>7</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>7</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>7</v>
@@ -1113,7 +1113,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>9</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>8</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -1174,42 +1174,42 @@
   <sheetData>
     <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>